<commit_message>
map.edf | remove weapon B armor B shield B npc
</commit_message>
<xml_diff>
--- a/gu_in/Map.edf/neutralC.xlsx
+++ b/gu_in/Map.edf/neutralC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\nexus-database-ce93b66d87acc5fafdd6979075eb27090fe3427e\nexus-database-ce93b66d87acc5fafdd6979075eb27090fe3427e\gu_in\Map.edf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\emay.dev\Parser_1.0.2\Database\gu_in\Map.edf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4AE4EA-A078-484C-BE9D-A55305992469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E9D70B-7C12-4AC9-848F-5925E6B77079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="18480" windowHeight="11205" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="18480" windowHeight="11205" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -46695,8 +46695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="D143" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="D124" sqref="D124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -49705,7 +49705,7 @@
         <v>8162</v>
       </c>
       <c r="D116" s="1">
-        <v>-138</v>
+        <v>-200138</v>
       </c>
       <c r="E116" s="1">
         <v>590</v>
@@ -49731,7 +49731,7 @@
         <v>8077</v>
       </c>
       <c r="D117" s="1">
-        <v>-140</v>
+        <v>-200140</v>
       </c>
       <c r="E117" s="1">
         <v>540</v>
@@ -49809,7 +49809,7 @@
         <v>8135</v>
       </c>
       <c r="D120" s="1">
-        <v>-136</v>
+        <v>-200136</v>
       </c>
       <c r="E120" s="1">
         <v>469</v>
@@ -49835,7 +49835,7 @@
         <v>8080</v>
       </c>
       <c r="D121" s="1">
-        <v>-142</v>
+        <v>-200142</v>
       </c>
       <c r="E121" s="1">
         <v>542</v>
@@ -49861,7 +49861,7 @@
         <v>8161</v>
       </c>
       <c r="D122" s="1">
-        <v>-136</v>
+        <v>-200136</v>
       </c>
       <c r="E122" s="1">
         <v>491</v>
@@ -49887,7 +49887,7 @@
         <v>8080</v>
       </c>
       <c r="D123" s="1">
-        <v>-142</v>
+        <v>-200142</v>
       </c>
       <c r="E123" s="1">
         <v>541</v>

</xml_diff>